<commit_message>
chore: update templates map and new M templates; CoC fixes; web app copies AM Tracker; docs updated
</commit_message>
<xml_diff>
--- a/maps/MBR Template Map.xlsx
+++ b/maps/MBR Template Map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AI Records\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Nguyen\Desktop\JobFolderCreation\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AF2E09-AE65-4336-9422-A348DE38A86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713BDBFB-F351-4CF2-A0D8-A77B215BDCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{B690BF04-EFDF-45E9-BA0E-0D7659FF5892}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
-  <si>
-    <t>Final Inspection</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">CofC for sterile </t>
   </si>
@@ -47,21 +44,6 @@
     <t>CofC for Non-Sterile</t>
   </si>
   <si>
-    <t>Document Type</t>
-  </si>
-  <si>
-    <t>Where Stored</t>
-  </si>
-  <si>
-    <t>CofC for Sterile</t>
-  </si>
-  <si>
-    <t>\S3D AI\AI Records\Empty Templates\Fake 825</t>
-  </si>
-  <si>
-    <t>Dim &amp; Meas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Item starts with A use: </t>
   </si>
   <si>
@@ -117,6 +99,12 @@
   </si>
   <si>
     <t>F-825-008Q S3D CofC (Carlsmed).docx</t>
+  </si>
+  <si>
+    <t>Item starts with M use:</t>
+  </si>
+  <si>
+    <t>F-825-1052C Inspection form CMD PN M.C00.00C.xlsx</t>
   </si>
 </sst>
 </file>
@@ -511,88 +499,92 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="22.68359375" customWidth="1"/>
-    <col min="2" max="2" width="28.3125" customWidth="1"/>
+    <col min="2" max="2" width="33.62890625" customWidth="1"/>
     <col min="3" max="3" width="26.578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -600,21 +592,13 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -628,47 +612,35 @@
       <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>4</v>
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>6</v>
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>6</v>
-      </c>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>6</v>
-      </c>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Web UI: progress + temp workspace build; config cleanup; templates handling; documentation updates
</commit_message>
<xml_diff>
--- a/maps/MBR Template Map.xlsx
+++ b/maps/MBR Template Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Nguyen\Desktop\JobFolderCreation\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713BDBFB-F351-4CF2-A0D8-A77B215BDCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCF2689-B567-4A39-813F-571C05C63524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{B690BF04-EFDF-45E9-BA0E-0D7659FF5892}"/>
   </bookViews>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C08E3922-EDD7-432C-99E8-35636E1A47FF}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -611,22 +611,10 @@
       <c r="B13" s="2"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>19</v>
-      </c>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>20</v>
-      </c>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -643,6 +631,22 @@
       <c r="B18" s="4"/>
       <c r="C18" s="2"/>
     </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update .gitignore to exclude temp Excel files and remove temporary web config file
</commit_message>
<xml_diff>
--- a/maps/MBR Template Map.xlsx
+++ b/maps/MBR Template Map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Nguyen\Desktop\JobFolderCreation-main\maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\WS Home-Team Folder\Document Control\QMS\ACTIVE QMS\825 - Monitoring &amp; Measurement\Carlsmed ( CMD)\JobFolderCreation-main\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B486DC78-1EAF-4FD8-BE88-4B4FB324BDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39483212-CED1-4BE2-BF09-4EB1C7E1C24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B690BF04-EFDF-45E9-BA0E-0D7659FF5892}"/>
+    <workbookView xWindow="28680" yWindow="-360" windowWidth="29040" windowHeight="15720" xr2:uid="{B690BF04-EFDF-45E9-BA0E-0D7659FF5892}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
     <t>F-825-1052E Inspection form CMD PN M.C00.00C_final.xlsx</t>
   </si>
   <si>
-    <t>F-825-247M CMD-C.L00.00.C LLIF Dimension Measure Rev 21_final_void.xlsx</t>
+    <t>F-825-247M CMD-C.L00.00.C LLIF Dimension Measure Rev 21_final.xlsx</t>
   </si>
 </sst>
 </file>
@@ -499,17 +499,17 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="67.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="67.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -520,7 +520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -531,7 +531,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -540,7 +540,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -551,7 +551,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -560,7 +560,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -569,7 +569,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -578,7 +578,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -587,51 +587,51 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,7 +639,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Add support for multi-letter prefixes in template mapping
- Update regex to extract multiple letters from 'Item starts with X use:' format
- Support prefixes like 'AMP', 'ASP' in addition to single letters
- Extract full prefix from item codes (e.g., 'AMP.123' extracts 'AMP')
- Maintain backward compatibility with single-letter prefixes
</commit_message>
<xml_diff>
--- a/maps/MBR Template Map.xlsx
+++ b/maps/MBR Template Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Nguyen\Desktop\JobFolderCreation-main\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD6815C-13DA-4348-B1CB-AB72BA56C126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5466B361-992A-416B-8B7B-54750EA29641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1815" windowWidth="21600" windowHeight="11295" xr2:uid="{B690BF04-EFDF-45E9-BA0E-0D7659FF5892}"/>
+    <workbookView xWindow="3345" yWindow="3105" windowWidth="21600" windowHeight="11295" xr2:uid="{B690BF04-EFDF-45E9-BA0E-0D7659FF5892}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t xml:space="preserve">CofC for sterile </t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>F-825-1052E Inspection form CMD PN M.C00.00C_final.xlsx</t>
+  </si>
+  <si>
+    <t>Item starts with AMP use:</t>
+  </si>
+  <si>
+    <t>Item starts with ASP use:</t>
+  </si>
+  <si>
+    <t>F-825-1100A CMD Final_In Process Inspection Template_final.xlsx</t>
   </si>
 </sst>
 </file>
@@ -496,7 +505,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,14 +591,22 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>

</xml_diff>